<commit_message>
Add interface of pack & unpack.
</commit_message>
<xml_diff>
--- a/doc/interface.xlsx
+++ b/doc/interface.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81002CA-3FAC-4196-9697-37710E927F8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE9CE78-92CC-448B-AA94-27A821030DB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
+    <sheet name="Pack" sheetId="2" r:id="rId2"/>
+    <sheet name="Unpack" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
   <si>
     <t>The Satellite Project Interface</t>
   </si>
@@ -32,13 +34,135 @@
   </si>
   <si>
     <t>https://localhost:8080/satellite</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Resource Name</t>
+  </si>
+  <si>
+    <t>Resource URL</t>
+  </si>
+  <si>
+    <t>Resource Files</t>
+  </si>
+  <si>
+    <t>Http Method</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Response Code</t>
+  </si>
+  <si>
+    <t>Response Body</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Failure</t>
+  </si>
+  <si>
+    <t>Bad Request</t>
+  </si>
+  <si>
+    <t>Failure Reasons</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>{apiRoot}/pack</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>type TNetsPack struct {
+	Src  []string `json:"src"`
+	Dest string   `json:"dest"`
+	Type string   `json:"type"`
+}</t>
+  </si>
+  <si>
+    <t>Request Body(Golang type)</t>
+  </si>
+  <si>
+    <t>Unprocessable Entity</t>
+  </si>
+  <si>
+    <t>Unpack</t>
+  </si>
+  <si>
+    <t>unpack</t>
+  </si>
+  <si>
+    <t>{apiRoot}/unpack</t>
+  </si>
+  <si>
+    <t>source files</t>
+  </si>
+  <si>
+    <t>dest file</t>
+  </si>
+  <si>
+    <t>type TNetsUnpack struct {
+	Src  string `json:"src"`
+	Dest string `json:"dest"`
+}</t>
+  </si>
+  <si>
+    <t>type TNetsUnpackVerboseReq struct {
+	Src string `json:"src"`
+}</t>
+  </si>
+  <si>
+    <t>{apiRoot}/unpack/f</t>
+  </si>
+  <si>
+    <t>{apiRoot}/unpack/m</t>
+  </si>
+  <si>
+    <t>type TNetsUnpackFileInfo struct {
+	Name string `json:"name"`
+	Size string `json:"size"`
+	Type string `json:"type"`
+}}</t>
+  </si>
+  <si>
+    <t>type TNetsUnpackToFile struct {
+	Src    string `json:"src"`
+	Target string `json:"target"`
+	Dest   string `json:"dest"`
+}</t>
+  </si>
+  <si>
+    <t>type TNetsUnpackToMemory struct {
+	Src    string `json:"src"`
+	Target string `json:"target"`
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +178,86 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -71,14 +265,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -363,7 +665,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -393,4 +695,510 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CFD4B1-235D-4E72-918F-F884BD21B93E}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" customWidth="1"/>
+    <col min="2" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="27.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" customWidth="1"/>
+    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8">
+        <v>200</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="11">
+        <v>400</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="11">
+        <v>422</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="11">
+        <v>500</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187E4885-EB28-4AF5-9943-3C8FB91CC162}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" customWidth="1"/>
+    <col min="2" max="5" width="18.1796875" customWidth="1"/>
+    <col min="6" max="6" width="27.26953125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" customWidth="1"/>
+    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8">
+        <v>200</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="11">
+        <v>400</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="11">
+        <v>422</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="11">
+        <v>500</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8">
+        <v>200</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="11">
+        <v>400</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="11">
+        <v>422</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="11">
+        <v>500</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="8">
+        <v>200</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="11">
+        <v>400</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="11">
+        <v>422</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="11">
+        <v>500</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="8">
+        <v>200</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="11">
+        <v>400</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="11">
+        <v>422</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="11">
+        <v>500</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change unpack verbose router.
</commit_message>
<xml_diff>
--- a/doc/interface.xlsx
+++ b/doc/interface.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE9CE78-92CC-448B-AA94-27A821030DB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6A0B69-8D67-4604-9422-A471688CFE8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t>The Satellite Project Interface</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>POST</t>
-  </si>
-  <si>
-    <t>o</t>
   </si>
   <si>
     <t>type TNetsPack struct {
@@ -156,6 +153,9 @@
 	Src    string `json:"src"`
 	Target string `json:"target"`
 }</t>
+  </si>
+  <si>
+    <t>{apiRoot}/unpack/v</t>
   </si>
 </sst>
 </file>
@@ -326,18 +326,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -347,19 +335,28 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -368,11 +365,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -664,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -732,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -745,78 +745,78 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="4">
         <v>200</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="10" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="6">
         <v>400</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="6">
         <v>422</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>25</v>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="11">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="6">
         <v>500</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -838,7 +838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187E4885-EB28-4AF5-9943-3C8FB91CC162}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F6" sqref="F6:F9"/>
     </sheetView>
   </sheetViews>
@@ -869,7 +869,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>9</v>
@@ -882,309 +882,301 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="4">
         <v>200</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="6"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="6">
         <v>400</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="6"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="20"/>
-      <c r="H4" s="11">
+      <c r="H4" s="6">
         <v>422</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>25</v>
+      <c r="I4" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="13"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="20"/>
-      <c r="H5" s="11">
+      <c r="H5" s="6">
         <v>500</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
-      <c r="C6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="17" t="s">
+      <c r="C6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="4">
         <v>200</v>
       </c>
-      <c r="I6" s="18" t="s">
-        <v>35</v>
+      <c r="I6" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="16"/>
       <c r="G7" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="6">
         <v>400</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="6"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="20"/>
-      <c r="H8" s="11">
+      <c r="H8" s="6">
         <v>422</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>25</v>
+      <c r="I8" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="20"/>
-      <c r="H9" s="11">
+      <c r="H9" s="6">
         <v>500</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="17" t="s">
+      <c r="C10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="4">
         <v>200</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="6"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="6">
         <v>400</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="21"/>
       <c r="B12" s="21"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="6"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="20"/>
-      <c r="H12" s="11">
+      <c r="H12" s="6">
         <v>422</v>
       </c>
-      <c r="I12" s="9" t="s">
-        <v>25</v>
+      <c r="I12" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="21"/>
       <c r="B13" s="21"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="11">
+      <c r="H13" s="6">
         <v>500</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="21"/>
       <c r="B14" s="21"/>
-      <c r="C14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="17" t="s">
+      <c r="C14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="F14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="4">
         <v>200</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="6"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="16"/>
       <c r="G15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="6">
         <v>400</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="20"/>
-      <c r="H16" s="11">
+      <c r="H16" s="6">
         <v>422</v>
       </c>
-      <c r="I16" s="9" t="s">
-        <v>25</v>
+      <c r="I16" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="20"/>
-      <c r="H17" s="11">
+      <c r="H17" s="6">
         <v>500</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="5" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B17"/>
     <mergeCell ref="G3:G5"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:D9"/>
@@ -1195,8 +1187,16 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G11:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change unpack file 'GET'->'POST'.
</commit_message>
<xml_diff>
--- a/doc/interface.xlsx
+++ b/doc/interface.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6A0B69-8D67-4604-9422-A471688CFE8E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A7560A-AB36-4A94-99D8-6CC5B21CFD47}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,16 +371,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187E4885-EB28-4AF5-9943-3C8FB91CC162}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -958,15 +958,15 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -983,11 +983,11 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="18"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="16"/>
       <c r="G7" s="19" t="s">
         <v>15</v>
@@ -1000,11 +1000,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="18"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="16"/>
       <c r="G8" s="20"/>
       <c r="H8" s="6">
@@ -1015,11 +1015,11 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="18"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="17"/>
       <c r="G9" s="20"/>
       <c r="H9" s="6">
@@ -1030,16 +1030,16 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>12</v>
+      <c r="E10" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>35</v>
@@ -1055,11 +1055,11 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="18"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="16"/>
       <c r="G11" s="19" t="s">
         <v>15</v>
@@ -1072,11 +1072,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="16"/>
       <c r="G12" s="20"/>
       <c r="H12" s="6">
@@ -1087,11 +1087,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="18"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="17"/>
       <c r="G13" s="20"/>
       <c r="H13" s="6">
@@ -1102,15 +1102,15 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="15" t="s">
@@ -1127,11 +1127,11 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="16"/>
       <c r="G15" s="19" t="s">
         <v>15</v>
@@ -1144,11 +1144,11 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="18"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="16"/>
       <c r="G16" s="20"/>
       <c r="H16" s="6">
@@ -1159,11 +1159,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="18"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="17"/>
       <c r="G17" s="20"/>
       <c r="H17" s="6">
@@ -1175,6 +1175,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G11:G13"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="G3:G5"/>
@@ -1191,12 +1197,6 @@
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G11:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update nets http interfaces document.
</commit_message>
<xml_diff>
--- a/doc/interface.xlsx
+++ b/doc/interface.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153D69F1-2635-41F3-9F67-2B4307FA70E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC968456-0530-453B-BAD0-C1058CB906D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
   <si>
     <t>The Satellite Project Interface</t>
   </si>
@@ -214,16 +214,34 @@
 	Type string `json:"type"`
 }</t>
   </si>
+  <si>
+    <t>type TNetsPackProcessReq struct {
+ Src  []string `json:"src"`
+ Type string   `json:"type"`
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>{apiRoot}/pack/p</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>type TNetsPackProcessResp struct {
+ Done int64 `json:"done"`
+ Work int64 `json:"work"`
+}</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -231,7 +249,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -239,28 +257,35 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -428,9 +453,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -438,10 +460,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,14 +750,14 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -740,12 +765,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8A1604E6-B58F-42AB-844F-6FF8C4AFAE33}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{F6A6D990-0D53-4122-B288-385ED77E48E0}"/>
@@ -756,23 +782,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CFD4B1-235D-4E72-918F-F884BD21B93E}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L10:L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="27.25" customWidth="1"/>
+    <col min="7" max="7" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -801,7 +827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>18</v>
       </c>
@@ -830,14 +856,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
       <c r="F3" s="16"/>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="6">
@@ -847,14 +873,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="14"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="6">
         <v>422</v>
       </c>
@@ -862,14 +888,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="14"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="10"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="6">
         <v>500</v>
       </c>
@@ -877,17 +903,96 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4">
+        <v>200</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6">
+        <v>400</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="6">
+        <v>422</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="6">
+        <v>500</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
+  <mergeCells count="12">
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="A2:A9"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -896,20 +1001,20 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E18" sqref="E18:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="27.25" customWidth="1"/>
+    <col min="7" max="7" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -938,7 +1043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>25</v>
       </c>
@@ -967,14 +1072,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="14"/>
       <c r="F3" s="16"/>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="6">
@@ -984,14 +1089,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="14"/>
       <c r="F4" s="16"/>
-      <c r="G4" s="20"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="6">
         <v>422</v>
       </c>
@@ -999,14 +1104,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="14"/>
       <c r="F5" s="17"/>
-      <c r="G5" s="20"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="6">
         <v>500</v>
       </c>
@@ -1014,16 +1119,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
+    <row r="6" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="15" t="s">
@@ -1039,14 +1144,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="18"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="6">
@@ -1056,14 +1161,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="18"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="6">
         <v>422</v>
       </c>
@@ -1071,14 +1176,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="18"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="17"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="6">
         <v>500</v>
       </c>
@@ -1086,16 +1191,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="116" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
+    <row r="10" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="13" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="15" t="s">
@@ -1111,14 +1216,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="18"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="6">
@@ -1128,14 +1233,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="20"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="6">
         <v>422</v>
       </c>
@@ -1143,14 +1248,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="18"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="6">
         <v>500</v>
       </c>
@@ -1158,9 +1263,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="13" t="s">
         <v>32</v>
       </c>
@@ -1183,14 +1288,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="14"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="6">
@@ -1200,14 +1305,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="6">
         <v>422</v>
       </c>
@@ -1215,14 +1320,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="14"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="6">
         <v>500</v>
       </c>
@@ -1230,16 +1335,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="13" t="s">
         <v>33</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="21" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="15" t="s">
@@ -1255,14 +1360,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
-      <c r="E19" s="18"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="6">
@@ -1272,14 +1377,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="18"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="20"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="6">
         <v>422</v>
       </c>
@@ -1287,14 +1392,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="18"/>
+      <c r="E21" s="21"/>
       <c r="F21" s="17"/>
-      <c r="G21" s="20"/>
+      <c r="G21" s="19"/>
       <c r="H21" s="6">
         <v>500</v>
       </c>
@@ -1304,12 +1409,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G11:G13"/>
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="B2:B21"/>
     <mergeCell ref="G3:G5"/>
@@ -1326,12 +1430,14 @@
     <mergeCell ref="D18:D21"/>
     <mergeCell ref="E18:E21"/>
     <mergeCell ref="F18:F21"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="G15:G17"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1345,17 +1451,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="27.25" customWidth="1"/>
+    <col min="7" max="7" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1384,7 +1490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>43</v>
       </c>
@@ -1413,7 +1519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -1430,7 +1536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
@@ -1445,7 +1551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
@@ -1470,6 +1576,7 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1478,21 +1585,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0D1F6C-9234-4549-AE3D-50046D768127}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="5" width="18.1796875" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" customWidth="1"/>
-    <col min="8" max="8" width="13.6328125" customWidth="1"/>
-    <col min="9" max="9" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="27.25" customWidth="1"/>
+    <col min="7" max="7" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1521,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
@@ -1550,7 +1657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
@@ -1567,7 +1674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
@@ -1582,7 +1689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13"/>
@@ -1607,6 +1714,7 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add document interfaces sheet.
</commit_message>
<xml_diff>
--- a/doc/interface.xlsx
+++ b/doc/interface.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EE650FF-50DE-44BA-8FA8-B72C9A5FC19F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57D5F83-47E0-4EAD-890E-A94C9CEB8C08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1310" yWindow="1900" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
-    <sheet name="Pack" sheetId="2" r:id="rId2"/>
-    <sheet name="Unpack" sheetId="3" r:id="rId3"/>
-    <sheet name="Comp" sheetId="4" r:id="rId4"/>
-    <sheet name="Decomp" sheetId="5" r:id="rId5"/>
+    <sheet name="Images" sheetId="6" r:id="rId2"/>
+    <sheet name="Pack" sheetId="2" r:id="rId3"/>
+    <sheet name="Unpack" sheetId="3" r:id="rId4"/>
+    <sheet name="Comp" sheetId="4" r:id="rId5"/>
+    <sheet name="Decomp" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -423,6 +424,19 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -438,20 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -781,10 +782,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A9DDCE-C680-4B31-B6FC-81081419A6A6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CFD4B1-235D-4E72-918F-F884BD21B93E}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -828,22 +841,22 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -857,13 +870,13 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="18"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="6">
@@ -874,13 +887,13 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="6">
         <v>422</v>
       </c>
@@ -889,13 +902,13 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="6">
         <v>500</v>
       </c>
@@ -904,18 +917,18 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="116">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="15" t="s">
         <v>52</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -929,13 +942,13 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="6">
@@ -946,13 +959,13 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="14"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="6">
         <v>422</v>
       </c>
@@ -961,13 +974,13 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="6">
         <v>500</v>
       </c>
@@ -976,18 +989,18 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="116">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="15" t="s">
         <v>52</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1001,13 +1014,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="13" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="6">
@@ -1018,13 +1031,13 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="6">
         <v>422</v>
       </c>
@@ -1033,13 +1046,13 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="6">
         <v>500</v>
       </c>
@@ -1049,6 +1062,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G3:G5"/>
     <mergeCell ref="G11:G13"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
@@ -1065,7 +1079,6 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
-    <mergeCell ref="G3:G5"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1073,7 +1086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187E4885-EB28-4AF5-9943-3C8FB91CC162}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -1121,22 +1134,22 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="15" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1150,13 +1163,13 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="18"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="13" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H3" s="6">
@@ -1167,13 +1180,13 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="6">
         <v>422</v>
       </c>
@@ -1182,13 +1195,13 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="6">
         <v>500</v>
       </c>
@@ -1197,18 +1210,18 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="130.5">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="8" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1222,13 +1235,13 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H7" s="6">
@@ -1239,13 +1252,13 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="14"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="6">
         <v>422</v>
       </c>
@@ -1254,13 +1267,13 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="6">
         <v>500</v>
       </c>
@@ -1269,18 +1282,18 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="130.5">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="15" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1294,13 +1307,13 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="13" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="6">
@@ -1311,13 +1324,13 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="14"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="6">
         <v>422</v>
       </c>
@@ -1326,13 +1339,13 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="14"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="6">
         <v>500</v>
       </c>
@@ -1341,18 +1354,18 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="116">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="8" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1366,13 +1379,13 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="13" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="6">
@@ -1383,13 +1396,13 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="14"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="6">
         <v>422</v>
       </c>
@@ -1398,13 +1411,13 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="6">
         <v>500</v>
       </c>
@@ -1413,18 +1426,18 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="8" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="15" t="s">
         <v>35</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1438,13 +1451,13 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="13" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H19" s="6">
@@ -1455,13 +1468,13 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="6">
         <v>422</v>
       </c>
@@ -1470,13 +1483,13 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="6">
         <v>500</v>
       </c>
@@ -1485,18 +1498,18 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="8" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="15" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -1510,13 +1523,13 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="13" t="s">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="6">
@@ -1527,13 +1540,13 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="14"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="6">
         <v>422</v>
       </c>
@@ -1542,13 +1555,13 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="14"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="6">
         <v>500</v>
       </c>
@@ -1558,19 +1571,7 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A2:A25"/>
-    <mergeCell ref="B2:B25"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="G3:G5"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="D10:D13"/>
@@ -1581,6 +1582,14 @@
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="G19:G21"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="E22:E25"/>
@@ -1589,7 +1598,11 @@
     <mergeCell ref="D14:D17"/>
     <mergeCell ref="E14:E17"/>
     <mergeCell ref="F14:F17"/>
-    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="A2:A25"/>
+    <mergeCell ref="B2:B25"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1597,7 +1610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F63A383-C4D6-48F5-85D8-DDBEA9F987FA}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -1645,22 +1658,22 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="15" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1674,12 +1687,12 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="18"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="19" t="s">
         <v>15</v>
       </c>
@@ -1691,12 +1704,12 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="20"/>
       <c r="H4" s="6">
         <v>422</v>
@@ -1706,12 +1719,12 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="21"/>
       <c r="H5" s="6">
         <v>500</v>
@@ -1735,7 +1748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0D1F6C-9234-4549-AE3D-50046D768127}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -1783,22 +1796,22 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="15" t="s">
         <v>51</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1812,12 +1825,12 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="18"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="19" t="s">
         <v>15</v>
       </c>
@@ -1829,12 +1842,12 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="20"/>
       <c r="H4" s="6">
         <v>422</v>
@@ -1844,12 +1857,12 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="18"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="12"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="21"/>
       <c r="H5" s="6">
         <v>500</v>

</xml_diff>